<commit_message>
hi i am punam
</commit_message>
<xml_diff>
--- a/First Test Scenario.xlsx
+++ b/First Test Scenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comp\Desktop\manual testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comp\Desktop\punamgit\Opencart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC3A5FE-0D68-4D75-898F-BC235AAF430E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A82983-09C9-4C86-A741-7FC01C325668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{48D7B60E-4659-45A9-B99D-1FE58B81FCE1}"/>
+    <workbookView xWindow="108" yWindow="2232" windowWidth="13056" windowHeight="8880" xr2:uid="{48D7B60E-4659-45A9-B99D-1FE58B81FCE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Project Name</t>
   </si>
@@ -134,6 +133,9 @@
   </si>
   <si>
     <t>ABC</t>
+  </si>
+  <si>
+    <t>Punam Bhoyar</t>
   </si>
 </sst>
 </file>
@@ -207,12 +209,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -228,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -549,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABE315C-85F1-470A-8993-5C6D32339AEA}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A2:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,202 +563,184 @@
     <col min="3" max="3" width="89.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>44798</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>44799</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="B15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="10" t="s">
+      <c r="B17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="B19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="B20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>